<commit_message>
Parte Casos de uso Excel Ale terminada
</commit_message>
<xml_diff>
--- a/Excels/Casos de uso.xlsx
+++ b/Excels/Casos de uso.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Nombre del caso de uso</t>
   </si>
@@ -37,13 +37,83 @@
     <t>Moverse (Guille)</t>
   </si>
   <si>
+    <t>El usuario puede hacer mover al personaje</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>1- La partida debe haber sido inicializada                                        2- El juego debe estar en estado jugable                                          3-El personaje no debe estar en estado recibiendo daño, o siendo agarrado o derribado por el enemigo</t>
+  </si>
+  <si>
+    <t>El personaje se ha movido a la dirección que ha querido el usuario</t>
+  </si>
+  <si>
+    <t>El personaje se mueve a la dirección correspondiente al botón que pulse el usuario</t>
+  </si>
+  <si>
+    <t>Si el personaje se mueve enfrente de un obstáculo interactuable, lo saltará automáticamente</t>
+  </si>
+  <si>
     <t>Login(Ale)</t>
+  </si>
+  <si>
+    <t>El usuario puede logearse</t>
+  </si>
+  <si>
+    <t>1- Dispone de cuenta para login         2- No hay error en el login                 3- Dispone conexión a internet</t>
+  </si>
+  <si>
+    <t>1- El usuario podrá crear partida.                                                    2- Cuándo la cree podrá guardar partida.                                                                              3- Cuándo inicie la partida, podrá crear una nueva o cargar partida.</t>
+  </si>
+  <si>
+    <t>1- El usuario crea cuenta.                2- Inicia juego.                                 3- Elige nueva partida o cargar partida.                                             4- Si crea nueva partida, puede elegir modo y dificultad.                   5- Si carga partida, elige cual quiere cargar.                                              6- Puede empezar el juego</t>
+  </si>
+  <si>
+    <t>1- Si no tiene cuenta no inicia juego.  2- Si tiene cuenta, pero no tiene partida guardada, tendrá que empezar una nueva.                         3- Si tiene partida guardada, puede o no empezar una nueva partida</t>
   </si>
   <si>
     <t>Controlar IA(César)</t>
   </si>
   <si>
+    <t>El sistema se encarga de la gestión de la IA de los enemigos, tanto de añadirlos al mapa como de gestionarlos y eliminarlos una vez muertos</t>
+  </si>
+  <si>
+    <t>Sistema, Jugador</t>
+  </si>
+  <si>
+    <t>1- La partida tiene que haberse cargado con éxito.                                              2- El jugador debe entrar en un area de combate.</t>
+  </si>
+  <si>
+    <t>1- El jugador tendrá menos recursos y balas.                                                2- El jugador podrá avanzar de zona.              3- Los enemigos derrotados desaparecerán liberando memoria para la siguiente zona.</t>
+  </si>
+  <si>
+    <t>1- El sistema generará a los enemigos previstos para la zona donde se encuentre el jugador.                            2- El sistema controla a los enemigos gestionando sus movimientos, visión, estado y coliciones.                                            3- Cuando la barra de vida de los enemigos baja a 0, el sistema los elimina del mapa para no colapsar la memoria.</t>
+  </si>
+  <si>
+    <t>En el paso 1 del flujo normal, si el jugador se encuentra en una zona libre de enemigos:                                                                                                                                                          1- El sistema no genera enemigos.                           2- El sistema se mantiene a la espera de que el jugador entre en una zona de combate.</t>
+  </si>
+  <si>
     <t>Gestion de niveles(Keliam)</t>
+  </si>
+  <si>
+    <t>El sistema comprueba que el jugador y la partida para que en caso necesario se pueda cambiar el nivel, por ejemplo al resolver un puzzle o si perdemos a nuestro compañero/a</t>
+  </si>
+  <si>
+    <t>1- Hay una partida cargada.
+2- El jugador completa una accion necesaria.
+3- Jefe muere.
+4- Compañero/a sale del nivel.</t>
+  </si>
+  <si>
+    <t>Cargara el nivel correspondiente tras completar la accion necesaria.</t>
+  </si>
+  <si>
+    <t>El usuario completa la accion establecida e informa al sistema para cargar el mapeado, el sistema cargara los elementos necesario del mapa, estructuras, enemigos, eventos. Lo renderiza y devuelve el control al usuario</t>
+  </si>
+  <si>
+    <t>1- Si el usuario ha muerto la zona de restaurará desde el último punto de control. restableciendo puzzles, enemigos y eventos.
+2- Si el compañero/a ha muerto se considera reinicio y pasa lo mismo que el caso anterior.</t>
   </si>
 </sst>
 </file>
@@ -114,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -130,14 +200,8 @@
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -406,16 +470,28 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" ht="61.5" customHeight="1">
+    <row r="2" ht="99.0" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -436,16 +512,28 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" ht="61.5" customHeight="1">
+    <row r="3" ht="114.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -466,16 +554,28 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" ht="61.5" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
+    <row r="4" ht="134.25" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -496,16 +596,28 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" ht="61.5" customHeight="1">
+    <row r="5" ht="86.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -529,7 +641,7 @@
     <row r="6" ht="61.5" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -556,7 +668,7 @@
     <row r="7" ht="61.5" customHeight="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -581,10 +693,10 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" ht="61.5" customHeight="1">
-      <c r="A8" s="9"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -612,7 +724,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>

</xml_diff>